<commit_message>
Fixed bugs with maneuvers displaying.
</commit_message>
<xml_diff>
--- a/Simulation_Setup.xlsx
+++ b/Simulation_Setup.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tyson\github\OrbitalManeuverVisualization\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tyson\github\OrbitalManeuverVisualization\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F913E1D-3F07-49EC-8730-5A9CF47503C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CACAAD5-B500-4EB7-93D5-63CE0E0ECE06}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-13995" yWindow="2445" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{E0547398-81EC-4442-B289-8539944A6DC5}"/>
+    <workbookView xWindow="46320" yWindow="2670" windowWidth="21600" windowHeight="11385" activeTab="2" xr2:uid="{E0547398-81EC-4442-B289-8539944A6DC5}"/>
   </bookViews>
   <sheets>
     <sheet name="Bodies" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="34">
   <si>
     <t>name</t>
   </si>
@@ -133,7 +133,13 @@
     <t>Plane Adjust</t>
   </si>
   <si>
-    <t>Transfer A</t>
+    <t>Insertion</t>
+  </si>
+  <si>
+    <t>Circularization</t>
+  </si>
+  <si>
+    <t>Transfer to Lunar Orbit</t>
   </si>
 </sst>
 </file>
@@ -640,7 +646,7 @@
   <dimension ref="A1:G9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -792,15 +798,15 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1E481B1B-DFE1-4187-9074-BE2B64D6C1C0}">
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.5703125" customWidth="1"/>
+    <col min="1" max="1" width="23.85546875" customWidth="1"/>
     <col min="3" max="3" width="12.5703125" customWidth="1"/>
     <col min="4" max="4" width="13.28515625" customWidth="1"/>
   </cols>
@@ -827,19 +833,19 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="B2" t="s">
         <v>2</v>
       </c>
       <c r="C2">
-        <v>100</v>
+        <v>3600</v>
       </c>
       <c r="D2">
-        <v>0</v>
+        <v>5310</v>
       </c>
       <c r="E2">
-        <v>400</v>
+        <v>0</v>
       </c>
       <c r="F2">
         <v>0</v>
@@ -847,21 +853,61 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B3" t="s">
         <v>2</v>
       </c>
       <c r="C3">
-        <v>101</v>
+        <v>7200</v>
       </c>
       <c r="D3">
-        <v>4000</v>
+        <v>0</v>
       </c>
       <c r="E3">
-        <v>0</v>
+        <v>-375</v>
       </c>
       <c r="F3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>31</v>
+      </c>
+      <c r="B4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4">
+        <v>357000</v>
+      </c>
+      <c r="D4">
+        <v>-850</v>
+      </c>
+      <c r="E4">
+        <v>0</v>
+      </c>
+      <c r="F4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>32</v>
+      </c>
+      <c r="B5" t="s">
+        <v>3</v>
+      </c>
+      <c r="C5">
+        <v>375000</v>
+      </c>
+      <c r="D5">
+        <v>-270</v>
+      </c>
+      <c r="E5">
+        <v>0</v>
+      </c>
+      <c r="F5">
         <v>0</v>
       </c>
     </row>

</xml_diff>